<commit_message>
gw: update TAS form
</commit_message>
<xml_diff>
--- a/LF/TAS/Guinee Bissau/gw_lf_tas1_3_fts_result_202206.xlsx
+++ b/LF/TAS/Guinee Bissau/gw_lf_tas1_3_fts_result_202206.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -3657,7 +3657,7 @@
     <t>allow_choice_duplicates</t>
   </si>
   <si>
-    <t>(Jun.2022).6..TAS1.FL.-.Resultado.FTS.V2</t>
+    <t>(Jun 2022) 6. TAS1 FL - Resultado FTS V2</t>
   </si>
   <si>
     <t>gw_lf_tas1_3_fts_result_202206_v2</t>
@@ -3672,9 +3672,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -3720,15 +3720,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3742,31 +3749,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3780,10 +3785,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3795,30 +3801,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3827,6 +3811,37 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3848,23 +3863,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3891,13 +3891,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3915,49 +3969,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3969,55 +4005,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4035,13 +4023,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4053,25 +4065,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4130,6 +4130,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -4141,6 +4150,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4168,199 +4212,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4383,9 +4383,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4781,7 +4778,7 @@
   <sheetPr/>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -4798,7 +4795,7 @@
     <col min="5" max="5" width="12.6222222222222" customWidth="1"/>
     <col min="6" max="6" width="16.8740740740741" customWidth="1"/>
     <col min="7" max="7" width="29.5037037037037" customWidth="1"/>
-    <col min="8" max="8" width="49.3777777777778" style="17" customWidth="1"/>
+    <col min="8" max="8" width="49.3777777777778" style="16" customWidth="1"/>
     <col min="9" max="9" width="12.6222222222222" customWidth="1"/>
     <col min="10" max="10" width="9.74814814814815" customWidth="1"/>
     <col min="11" max="11" width="35.3777777777778" customWidth="1"/>
@@ -4807,43 +4804,43 @@
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="1" ht="36" spans="1:14">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -4851,359 +4848,359 @@
       </c>
     </row>
     <row r="2" s="3" customFormat="1" ht="42.75" spans="1:13">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="20"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:13">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="20"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:13">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="20" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:13">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="20" t="s">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:13">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="20" t="s">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:13">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="32" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:13">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="21" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="32" t="s">
+      <c r="I8" s="20"/>
+      <c r="J8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="42.75" spans="1:13">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="35" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="32" t="s">
+      <c r="I9" s="20"/>
+      <c r="J9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:13">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="21" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="32" t="s">
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="20"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:13">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="32" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:13">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="25" t="s">
+      <c r="D12" s="26"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="32" t="s">
+      <c r="I12" s="20"/>
+      <c r="J12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:13">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="25" t="s">
+      <c r="D13" s="26"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="32" t="s">
+      <c r="I13" s="20"/>
+      <c r="J13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:13">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="20" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="57" spans="1:13">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="25" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" s="3" customFormat="1" spans="1:13">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -5213,26 +5210,26 @@
         <v>74</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="32" t="s">
+      <c r="I16" s="19"/>
+      <c r="J16" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -5247,11 +5244,11 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="24" t="s">
         <v>72</v>
       </c>
       <c r="I17" s="8"/>
-      <c r="J17" s="32" t="s">
+      <c r="J17" s="31" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="8"/>
@@ -5259,7 +5256,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -5272,11 +5269,11 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="24" t="s">
         <v>79</v>
       </c>
       <c r="I18" s="8"/>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="31" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="8"/>
@@ -5284,7 +5281,7 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -5297,11 +5294,11 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>81</v>
       </c>
       <c r="I19" s="8"/>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="31" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="8"/>
@@ -5309,7 +5306,7 @@
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -5320,10 +5317,10 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>68</v>
       </c>
       <c r="J20" s="8"/>
@@ -5331,50 +5328,50 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" s="16" customFormat="1" spans="1:13">
-      <c r="A21" s="20" t="s">
+    <row r="21" s="15" customFormat="1" spans="1:13">
+      <c r="A21" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="28" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-    </row>
-    <row r="22" s="17" customFormat="1" spans="1:13">
-      <c r="A22" s="25" t="s">
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+    </row>
+    <row r="22" s="16" customFormat="1" spans="1:13">
+      <c r="A22" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -5387,7 +5384,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="24" t="s">
         <v>89</v>
       </c>
       <c r="I23" s="8"/>
@@ -5397,7 +5394,7 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -5410,7 +5407,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="30"/>
+      <c r="H24" s="29"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -5418,7 +5415,7 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -5429,7 +5426,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="30"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -5437,7 +5434,7 @@
       <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>94</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -5448,7 +5445,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="30"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -5669,7 +5666,7 @@
       <c r="C17" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18" s="4" customFormat="1" spans="1:5">
@@ -5682,7 +5679,7 @@
       <c r="C18" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" s="4" customFormat="1" spans="1:5">
@@ -5695,7 +5692,7 @@
       <c r="C19" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="11"/>
     </row>
     <row r="20" s="4" customFormat="1" spans="1:5">
@@ -5708,7 +5705,7 @@
       <c r="C20" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="11"/>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
@@ -5721,14 +5718,14 @@
       <c r="C21" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22" s="4" customFormat="1" spans="1:5">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="11"/>
     </row>
     <row r="23" s="4" customFormat="1" spans="1:5">
@@ -5741,7 +5738,7 @@
       <c r="C23" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E23" s="11"/>
@@ -5756,7 +5753,7 @@
       <c r="C24" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E24" s="11"/>
@@ -5771,7 +5768,7 @@
       <c r="C25" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E25" s="11"/>
@@ -5780,796 +5777,796 @@
       <c r="A26" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" s="4" customFormat="1" spans="1:5">
       <c r="A27" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" s="4" customFormat="1" spans="1:5">
       <c r="A28" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="15"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" s="4" customFormat="1" spans="1:5">
       <c r="A29" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="15"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" s="4" customFormat="1" spans="1:5">
       <c r="A30" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="14"/>
     </row>
     <row r="31" s="4" customFormat="1" spans="1:5">
       <c r="A31" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="15"/>
+      <c r="E31" s="14"/>
     </row>
     <row r="32" s="4" customFormat="1" spans="1:5">
       <c r="A32" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="14"/>
     </row>
     <row r="33" s="4" customFormat="1" spans="1:5">
       <c r="A33" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="14"/>
     </row>
     <row r="34" s="4" customFormat="1" spans="1:5">
       <c r="A34" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="15"/>
+      <c r="E34" s="14"/>
     </row>
     <row r="35" s="4" customFormat="1" spans="1:5">
       <c r="A35" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" s="4" customFormat="1" spans="1:5">
       <c r="A36" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="14"/>
     </row>
     <row r="37" s="4" customFormat="1" spans="1:5">
       <c r="A37" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E37" s="15"/>
+      <c r="E37" s="14"/>
     </row>
     <row r="38" s="4" customFormat="1" spans="1:5">
       <c r="A38" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E38" s="15"/>
+      <c r="E38" s="14"/>
     </row>
     <row r="39" s="4" customFormat="1" spans="1:5">
       <c r="A39" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="14"/>
     </row>
     <row r="40" s="4" customFormat="1" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E40" s="15"/>
+      <c r="E40" s="14"/>
     </row>
     <row r="41" s="4" customFormat="1" spans="1:5">
       <c r="A41" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="15"/>
+      <c r="E41" s="14"/>
     </row>
     <row r="42" s="4" customFormat="1" spans="1:5">
       <c r="A42" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E42" s="15"/>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" s="4" customFormat="1" spans="1:5">
       <c r="A43" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="15"/>
+      <c r="E43" s="14"/>
     </row>
     <row r="44" s="4" customFormat="1" spans="1:5">
       <c r="A44" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E44" s="15"/>
+      <c r="E44" s="14"/>
     </row>
     <row r="45" s="4" customFormat="1" spans="1:5">
       <c r="A45" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E45" s="15"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" s="4" customFormat="1" spans="1:5">
       <c r="A46" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E46" s="15"/>
+      <c r="E46" s="14"/>
     </row>
     <row r="47" s="4" customFormat="1" spans="1:5">
       <c r="A47" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E47" s="15"/>
+      <c r="E47" s="14"/>
     </row>
     <row r="48" s="4" customFormat="1" spans="1:5">
       <c r="A48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E48" s="15"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" s="4" customFormat="1" spans="1:5">
       <c r="A49" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E49" s="15"/>
+      <c r="E49" s="14"/>
     </row>
     <row r="50" s="4" customFormat="1" spans="1:5">
       <c r="A50" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E50" s="15"/>
+      <c r="E50" s="14"/>
     </row>
     <row r="51" s="4" customFormat="1" spans="1:5">
       <c r="A51" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="15"/>
+      <c r="E51" s="14"/>
     </row>
     <row r="52" s="4" customFormat="1" spans="1:5">
       <c r="A52" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E52" s="15"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" s="4" customFormat="1" spans="1:5">
       <c r="A53" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E53" s="15"/>
+      <c r="E53" s="14"/>
     </row>
     <row r="54" s="4" customFormat="1" spans="1:5">
       <c r="A54" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E54" s="15"/>
+      <c r="E54" s="14"/>
     </row>
     <row r="55" s="4" customFormat="1" spans="1:5">
       <c r="A55" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E55" s="15"/>
+      <c r="E55" s="14"/>
     </row>
     <row r="56" s="4" customFormat="1" spans="1:5">
       <c r="A56" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E56" s="15"/>
+      <c r="E56" s="14"/>
     </row>
     <row r="57" s="4" customFormat="1" spans="1:5">
       <c r="A57" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="15"/>
+      <c r="E57" s="14"/>
     </row>
     <row r="58" s="4" customFormat="1" spans="1:5">
       <c r="A58" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E58" s="15"/>
+      <c r="E58" s="14"/>
     </row>
     <row r="59" s="4" customFormat="1" spans="1:5">
       <c r="A59" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E59" s="15"/>
+      <c r="E59" s="14"/>
     </row>
     <row r="60" s="4" customFormat="1" spans="1:5">
       <c r="A60" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E60" s="15"/>
+      <c r="E60" s="14"/>
     </row>
     <row r="61" s="4" customFormat="1" spans="1:5">
       <c r="A61" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E61" s="15"/>
+      <c r="E61" s="14"/>
     </row>
     <row r="62" s="4" customFormat="1" spans="1:5">
       <c r="A62" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E62" s="15"/>
+      <c r="E62" s="14"/>
     </row>
     <row r="63" s="4" customFormat="1" spans="1:5">
       <c r="A63" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E63" s="15"/>
+      <c r="E63" s="14"/>
     </row>
     <row r="64" s="4" customFormat="1" spans="1:5">
       <c r="A64" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="15"/>
+      <c r="E64" s="14"/>
     </row>
     <row r="65" s="4" customFormat="1" spans="1:5">
       <c r="A65" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E65" s="15"/>
+      <c r="E65" s="14"/>
     </row>
     <row r="66" s="4" customFormat="1" spans="1:5">
       <c r="A66" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E66" s="15"/>
+      <c r="E66" s="14"/>
     </row>
     <row r="67" s="4" customFormat="1" spans="1:5">
       <c r="A67" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E67" s="15"/>
+      <c r="E67" s="14"/>
     </row>
     <row r="68" s="4" customFormat="1" spans="1:5">
       <c r="A68" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E68" s="15"/>
+      <c r="E68" s="14"/>
     </row>
     <row r="69" s="4" customFormat="1" spans="1:5">
       <c r="A69" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E69" s="15"/>
+      <c r="E69" s="14"/>
     </row>
     <row r="70" s="4" customFormat="1" spans="1:5">
       <c r="A70" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E70" s="15"/>
+      <c r="E70" s="14"/>
     </row>
     <row r="71" s="4" customFormat="1" spans="1:5">
       <c r="A71" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D71" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E71" s="15"/>
+      <c r="E71" s="14"/>
     </row>
     <row r="72" s="4" customFormat="1" spans="1:5">
       <c r="A72" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D72" s="15" t="s">
+      <c r="D72" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E72" s="15"/>
+      <c r="E72" s="14"/>
     </row>
     <row r="73" s="4" customFormat="1" spans="1:5">
       <c r="A73" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="C73" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E73" s="15"/>
+      <c r="E73" s="14"/>
     </row>
     <row r="74" s="4" customFormat="1" spans="1:5">
       <c r="A74" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="15"/>
+      <c r="E74" s="14"/>
     </row>
     <row r="75" s="4" customFormat="1" spans="1:5">
       <c r="A75" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="C75" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E75" s="15"/>
+      <c r="E75" s="14"/>
     </row>
     <row r="76" s="4" customFormat="1" spans="1:5">
       <c r="A76" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="C76" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="D76" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E76" s="15"/>
+      <c r="E76" s="14"/>
     </row>
     <row r="77" s="4" customFormat="1" spans="1:5">
       <c r="A77" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C77" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D77" s="15" t="s">
+      <c r="D77" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E77" s="15"/>
+      <c r="E77" s="14"/>
     </row>
     <row r="78" s="4" customFormat="1" spans="1:5">
       <c r="A78" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="C78" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="D78" s="15" t="s">
+      <c r="D78" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E78" s="15"/>
+      <c r="E78" s="14"/>
     </row>
     <row r="79" customFormat="1" spans="1:1">
       <c r="A79" s="11"/>
@@ -35346,8 +35343,8 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>

</xml_diff>